<commit_message>
build pm data for 2020-06-20
</commit_message>
<xml_diff>
--- a/data/source/kc_county_breakdowns/KCMO COVID-19 Data by County.xlsx
+++ b/data/source/kc_county_breakdowns/KCMO COVID-19 Data by County.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Community Engagement\2020 Data Requested\(6)June\COVID19 by County Request\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prenercg/GitHub/openGIS/covid_daily_viz/data/source/kc_county_breakdowns/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D9EB609-4F0E-4625-A195-F6850EA7D3AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA84823-1D0B-D144-AD29-8AACB898A6F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{273B6D85-80F8-4B9A-A275-40EE0CF9F652}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{273B6D85-80F8-4B9A-A275-40EE0CF9F652}"/>
   </bookViews>
   <sheets>
     <sheet name="KCMO COVID19 by County" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,15 +326,15 @@
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.6328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="17" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -351,7 +351,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>43913</v>
       </c>
@@ -368,7 +368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>43914</v>
       </c>
@@ -385,7 +385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>43915</v>
       </c>
@@ -402,7 +402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>43916</v>
       </c>
@@ -419,7 +419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>43917</v>
       </c>
@@ -436,7 +436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>43920</v>
       </c>
@@ -453,7 +453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>43921</v>
       </c>
@@ -470,7 +470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>43922</v>
       </c>
@@ -487,7 +487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>43923</v>
       </c>
@@ -504,7 +504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>43924</v>
       </c>
@@ -521,7 +521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>43927</v>
       </c>
@@ -538,7 +538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>43928</v>
       </c>
@@ -555,7 +555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>43929</v>
       </c>
@@ -572,7 +572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>43930</v>
       </c>
@@ -589,7 +589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>43931</v>
       </c>
@@ -606,7 +606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>43934</v>
       </c>
@@ -623,7 +623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>43936</v>
       </c>
@@ -640,7 +640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>43937</v>
       </c>
@@ -657,7 +657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>43938</v>
       </c>
@@ -674,17 +674,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>43939</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>43940</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="1">
         <v>43941</v>
       </c>
@@ -701,7 +701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="1">
         <v>43942</v>
       </c>
@@ -718,7 +718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="1">
         <v>43943</v>
       </c>
@@ -735,7 +735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="1">
         <v>43944</v>
       </c>
@@ -752,7 +752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="1">
         <v>43945</v>
       </c>
@@ -769,17 +769,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="1">
         <v>43946</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="1">
         <v>43947</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="1">
         <v>43948</v>
       </c>
@@ -796,7 +796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="1">
         <v>43949</v>
       </c>
@@ -813,7 +813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="1">
         <v>43950</v>
       </c>
@@ -830,7 +830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="1">
         <v>43951</v>
       </c>
@@ -847,7 +847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="1">
         <v>43952</v>
       </c>
@@ -864,17 +864,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="1">
         <v>43953</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="1">
         <v>43954</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="1">
         <v>43955</v>
       </c>
@@ -891,7 +891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="1">
         <v>43956</v>
       </c>
@@ -908,7 +908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="1">
         <v>43957</v>
       </c>
@@ -925,7 +925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="1">
         <v>43958</v>
       </c>
@@ -942,7 +942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="1">
         <v>43959</v>
       </c>
@@ -959,7 +959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="1">
         <v>43962</v>
       </c>
@@ -976,7 +976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="1">
         <v>43963</v>
       </c>
@@ -993,7 +993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="1">
         <v>43964</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="1">
         <v>43965</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="1">
         <v>43966</v>
       </c>
@@ -1044,17 +1044,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="1">
         <v>43967</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" s="1">
         <v>43968</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" s="1">
         <v>43969</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="1">
         <v>43970</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" s="1">
         <v>43971</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="1">
         <v>43972</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="1">
         <v>43973</v>
       </c>
@@ -1139,22 +1139,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="1">
         <v>43974</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="1">
         <v>43975</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="1">
         <v>43976</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" s="1">
         <v>43977</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="1">
         <v>43978</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="1">
         <v>43979</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="A60" s="1">
         <v>43980</v>
       </c>
@@ -1222,17 +1222,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="1">
         <v>43981</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" s="1">
         <v>43982</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" s="1">
         <v>43983</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" s="1">
         <v>43984</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="1">
         <v>43985</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="1">
         <v>43986</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="1">
         <v>43987</v>
       </c>
@@ -1317,17 +1317,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" s="1">
         <v>43988</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" s="1">
         <v>43989</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" s="1">
         <v>43990</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" s="1">
         <v>43991</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" s="1">
         <v>43992</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" s="1">
         <v>43993</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" s="1">
         <v>43994</v>
       </c>
@@ -1412,17 +1412,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5">
       <c r="A75" s="1">
         <v>43995</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" s="1">
         <v>43996</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" s="1">
         <v>43997</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" s="1">
         <v>43998</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" s="1">
         <v>43999</v>
       </c>

</xml_diff>